<commit_message>
edited harp doc validation file DOCwc
</commit_message>
<xml_diff>
--- a/HarpLake/HarpValidationDOC.xlsx
+++ b/HarpLake/HarpValidationDOC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IADO\GLEN Fellowship Program\GFP 1\SOS\HarpLake\1991-2001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\SOS\HarpLake\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>datetime</t>
   </si>
   <si>
     <t>DOC</t>
+  </si>
+  <si>
+    <t>DOCwc</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -362,971 +365,1334 @@
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>33259</v>
       </c>
       <c r="B2">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>33296</v>
       </c>
       <c r="B3">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>33317</v>
       </c>
       <c r="B4">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>33345</v>
       </c>
       <c r="B5">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>33352</v>
       </c>
       <c r="B6">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>33359</v>
       </c>
       <c r="B7">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>33371</v>
       </c>
       <c r="B8">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.7</v>
+      </c>
+      <c r="C8">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>33380</v>
       </c>
       <c r="B9">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.7</v>
+      </c>
+      <c r="C9">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>33394</v>
       </c>
       <c r="B10">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+      <c r="C10">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>33408</v>
       </c>
       <c r="B11">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C11">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>33427</v>
       </c>
       <c r="B12">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>33441</v>
       </c>
       <c r="B13">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="C13">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>33456</v>
       </c>
       <c r="B14">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.9</v>
+      </c>
+      <c r="C14">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>33472</v>
       </c>
       <c r="B15">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>33486</v>
       </c>
       <c r="B16">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C16">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>33498</v>
       </c>
       <c r="B17">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+      <c r="C17">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>33512</v>
       </c>
       <c r="B18">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+      <c r="C18">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>33527</v>
       </c>
       <c r="B19">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+      <c r="C19">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>33541</v>
       </c>
       <c r="B20">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.9</v>
+      </c>
+      <c r="C20">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>33556</v>
       </c>
       <c r="B21">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>33625</v>
       </c>
       <c r="B22">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>33661</v>
       </c>
       <c r="B23">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>33700</v>
       </c>
       <c r="B24">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>33731</v>
       </c>
       <c r="B25">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>33763</v>
       </c>
       <c r="B26">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+      <c r="C26">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>33813</v>
       </c>
       <c r="B27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>33842</v>
       </c>
       <c r="B28">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C28">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>33864</v>
       </c>
       <c r="B29">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="C29">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>33891</v>
       </c>
       <c r="B30">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C30">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>33924</v>
       </c>
       <c r="B31">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>34010</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>34067</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>34087</v>
       </c>
       <c r="B34">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34109</v>
       </c>
       <c r="B35">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C35">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34149</v>
       </c>
       <c r="B36">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C36">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>34192</v>
       </c>
       <c r="B37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>34227</v>
       </c>
       <c r="B38">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="C38">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>34260.413194444402</v>
       </c>
       <c r="B39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>34288</v>
       </c>
       <c r="B40">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>34458</v>
       </c>
       <c r="B41">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>34500</v>
       </c>
       <c r="B42">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.9</v>
+      </c>
+      <c r="C42">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>34536</v>
       </c>
       <c r="B43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>34555</v>
       </c>
       <c r="B44">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="C44">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>34591</v>
       </c>
       <c r="B45">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C45">
         <v>4.2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>34631</v>
       </c>
       <c r="B46">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C46">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>34809</v>
       </c>
       <c r="B47">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>34843</v>
       </c>
       <c r="B48">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>34871</v>
       </c>
       <c r="B49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.2</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>34933</v>
       </c>
       <c r="B50">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5.3</v>
+      </c>
+      <c r="C50">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>34963</v>
       </c>
       <c r="B51">
+        <v>5.2</v>
+      </c>
+      <c r="C51">
         <v>4.3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>35010</v>
       </c>
       <c r="B52">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>35192</v>
       </c>
       <c r="B53">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>35227</v>
       </c>
       <c r="B54">
+        <v>5.2</v>
+      </c>
+      <c r="C54">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>35257.5</v>
       </c>
       <c r="B55">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C55">
         <v>4.2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>35298</v>
       </c>
       <c r="B56">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C56">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>35319</v>
       </c>
       <c r="B57">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.8</v>
+      </c>
+      <c r="C57">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>35347</v>
       </c>
       <c r="B58">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>35556</v>
       </c>
       <c r="B59">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>35593</v>
       </c>
       <c r="B60">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.7</v>
+      </c>
+      <c r="C60">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>35621</v>
       </c>
       <c r="B61">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>35649</v>
       </c>
       <c r="B62">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.9</v>
+      </c>
+      <c r="C62">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>35688</v>
       </c>
       <c r="B63">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>35733</v>
       </c>
       <c r="B64">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>35905</v>
       </c>
       <c r="B65">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>35922</v>
       </c>
       <c r="B66">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>35936</v>
       </c>
       <c r="B67">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>35951</v>
       </c>
       <c r="B68">
+        <v>3.6</v>
+      </c>
+      <c r="C68">
         <v>3.4</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>35962</v>
       </c>
       <c r="B69">
+        <v>3.6</v>
+      </c>
+      <c r="C69">
         <v>3.5</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>35976</v>
       </c>
       <c r="B70">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.9</v>
+      </c>
+      <c r="C70">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>35990</v>
       </c>
       <c r="B71">
+        <v>3.7</v>
+      </c>
+      <c r="C71">
         <v>3.5</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>36019</v>
       </c>
       <c r="B72">
+        <v>3.7</v>
+      </c>
+      <c r="C72">
         <v>3.5</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>36034</v>
       </c>
       <c r="B73">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.9</v>
+      </c>
+      <c r="C73">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>36055</v>
       </c>
       <c r="B74">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+      <c r="C74">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>36073</v>
       </c>
       <c r="B75">
+        <v>3.7</v>
+      </c>
+      <c r="C75">
         <v>3.5</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>36094</v>
       </c>
       <c r="B76">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>36266</v>
       </c>
       <c r="B77">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>36284</v>
       </c>
       <c r="B78">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>36291</v>
       </c>
       <c r="B79">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>36307</v>
       </c>
       <c r="B80">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.7</v>
+      </c>
+      <c r="C80">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>36321</v>
       </c>
       <c r="B81">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C81">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>36328</v>
       </c>
       <c r="B82">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C82">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>36341</v>
       </c>
       <c r="B83">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C83">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>36354</v>
       </c>
       <c r="B84">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C84">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>36369</v>
       </c>
       <c r="B85">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C85">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>36382</v>
       </c>
       <c r="B86">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C86">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>36396</v>
       </c>
       <c r="B87">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C87">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>36416</v>
       </c>
       <c r="B88">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.2</v>
+      </c>
+      <c r="C88">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>36430</v>
       </c>
       <c r="B89">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C89">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>36447</v>
       </c>
       <c r="B90">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C90">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>36468</v>
       </c>
       <c r="B91">
+        <v>4</v>
+      </c>
+      <c r="C91">
         <v>3.4</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>36635</v>
       </c>
       <c r="B92">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>36657</v>
       </c>
       <c r="B93">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C93">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>36670</v>
       </c>
       <c r="B94">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C94">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>36683</v>
       </c>
       <c r="B95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>36699</v>
       </c>
       <c r="B96">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C96">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>36711</v>
       </c>
       <c r="B97">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.7</v>
+      </c>
+      <c r="C97">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>36725</v>
       </c>
       <c r="B98">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C98">
         <v>4.3</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>36740</v>
       </c>
       <c r="B99">
+        <v>4.8</v>
+      </c>
+      <c r="C99">
         <v>4.3</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>36754</v>
       </c>
       <c r="B100">
+        <v>5.2</v>
+      </c>
+      <c r="C100">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>36767</v>
       </c>
       <c r="B101">
+        <v>5</v>
+      </c>
+      <c r="C101">
         <v>4.2</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>36782</v>
       </c>
       <c r="B102">
+        <v>5</v>
+      </c>
+      <c r="C102">
         <v>4.3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>36794</v>
       </c>
       <c r="B103">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>36809</v>
       </c>
       <c r="B104">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C104">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>36825</v>
       </c>
       <c r="B105">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C105">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>36857</v>
       </c>
       <c r="B106">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>37018</v>
       </c>
       <c r="B107">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>37036</v>
       </c>
       <c r="B108">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>37047</v>
       </c>
       <c r="B109">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="C109">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>37062</v>
       </c>
       <c r="B110">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C110">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>37075</v>
       </c>
       <c r="B111">
+        <v>4.8</v>
+      </c>
+      <c r="C111">
         <v>4.3</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>37090</v>
       </c>
       <c r="B112">
+        <v>4.8</v>
+      </c>
+      <c r="C112">
         <v>4.3</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>37105</v>
       </c>
       <c r="B113">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C113">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>37117</v>
       </c>
       <c r="B114">
+        <v>4.7</v>
+      </c>
+      <c r="C114">
         <v>4.2</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>37131</v>
       </c>
       <c r="B115">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.2</v>
+      </c>
+      <c r="C115">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>37146</v>
       </c>
       <c r="B116">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>37161</v>
       </c>
       <c r="B117">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C117">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>37173</v>
       </c>
       <c r="B118">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C118">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>37188</v>
       </c>
       <c r="B119">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="C119">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>37200</v>
       </c>
       <c r="B120">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C120">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>37225</v>
       </c>
       <c r="B121">
+        <v>4.2</v>
+      </c>
+      <c r="C121">
         <v>4.2</v>
       </c>
     </row>

</xml_diff>